<commit_message>
add test case tk doanh thu
</commit_message>
<xml_diff>
--- a/Đợt 4/CTS6326_Test cases.xlsx
+++ b/Đợt 4/CTS6326_Test cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DH-CNTT\Môn thay thế\Kỹ thuật lập trình hướng đối tượng\project\BlockBusterDoc\Đợt 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DH-CNTT\Môn thay thế\Kỹ thuật lập trình hướng đối tượng\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003618D2-FDEF-4D7C-9AA2-44DCCB1F3675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B41CE22-8C18-4D94-BBCA-E464B66C8D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1784" uniqueCount="416">
   <si>
     <t>Thiết kế</t>
   </si>
@@ -746,9 +746,6 @@
     <t>MovieCast( Robert Downey Jr)</t>
   </si>
   <si>
-    <t>Diễn viên được xóa khỏi danh sách diễn viên trong phim và thêm vào danh sách diễn viên chưa có trong phim</t>
-  </si>
-  <si>
     <t>Danh sách diễn viên có và chưa có trong phim</t>
   </si>
   <si>
@@ -758,9 +755,6 @@
     <t>MovieCast( Robert Downey Jr, Abraham)</t>
   </si>
   <si>
-    <t>Diễn viên được xóa khỏi danh sách diễn viên chưa có trong phim và thêm vào danh sách diễn viên có trong phim</t>
-  </si>
-  <si>
     <t>Quản lí đạo diễn</t>
   </si>
   <si>
@@ -900,6 +894,9 @@
   </si>
   <si>
     <t>Thông báo: Đăng ký thất bại!!! Email đã có người sử dụng!</t>
+  </si>
+  <si>
+    <t>(Trương, Hiền, 26/06/2000, Nam, Đồng Tháp, Tháp Mười, Thanh Mỹ, tnthien.cdr@gmail.com,  trunghiendk, 1234,1234)</t>
   </si>
   <si>
     <t>trunghiendk, 1234</t>
@@ -1252,10 +1249,40 @@
     <t>trunghienuser, 1234</t>
   </si>
   <si>
-    <t>(Trương, Hiền, 26/06/2000, Nam, Đồng Tháp, Tháp Mười, Thanh Mỹ, duylong3596@gmail.com,  trunghiendk, 1234,1234)</t>
-  </si>
-  <si>
-    <t>vonguyenduylong92.1415@gmail.com</t>
+    <t>Thống kê doanh thu</t>
+  </si>
+  <si>
+    <t>Tổng doanh thu từ trước đến giờ</t>
+  </si>
+  <si>
+    <t>Chỉ nhập ngày bắt đầu</t>
+  </si>
+  <si>
+    <t>Doanh thu từ ngày bắt đầu đến hiện tại</t>
+  </si>
+  <si>
+    <t>Chỉ nhập ngày kết thúc</t>
+  </si>
+  <si>
+    <t>18/10/2023</t>
+  </si>
+  <si>
+    <t>Doanh thu từ trước đến giờ đến ngày kết thúc</t>
+  </si>
+  <si>
+    <t>Ngày kết thúc bé hơn ngày bắt đầu</t>
+  </si>
+  <si>
+    <t>(18/10/2023, 1/10/2023)</t>
+  </si>
+  <si>
+    <t>Thông báo: Từ ngày ngày không thể sau đến ngày!!!</t>
+  </si>
+  <si>
+    <t>Thông báo: Xoá thành công!!! Và Diễn viên được xóa khỏi danh sách diễn viên trong phim và thêm vào danh sách diễn viên chưa có trong phim</t>
+  </si>
+  <si>
+    <t>Hiển thị hộp thoại nhập vai diễn. Bấm OK -&gt; Diễn viên được xóa khỏi danh sách diễn viên chưa có trong phim và thêm vào danh sách diễn viên có trong phim</t>
   </si>
 </sst>
 </file>
@@ -1426,7 +1453,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
@@ -1839,10 +1866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F357"/>
+  <dimension ref="A2:F363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="112" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="A206" zoomScale="112" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E215" sqref="E215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2007,7 +2034,7 @@
         <v>39</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F12" s="3"/>
     </row>
@@ -2022,7 +2049,7 @@
         <v>40</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F13" s="13"/>
     </row>
@@ -2037,7 +2064,7 @@
         <v>175</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -2049,7 +2076,7 @@
         <v>36</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>405</v>
+        <v>287</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>41</v>
@@ -2106,7 +2133,7 @@
         <v>12</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F19" s="3"/>
     </row>
@@ -2133,7 +2160,7 @@
         <v>107</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>108</v>
@@ -2145,13 +2172,13 @@
         <v>3.5</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F22" s="11"/>
     </row>
@@ -2205,7 +2232,7 @@
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F26" s="3"/>
     </row>
@@ -2220,7 +2247,7 @@
         <v>44</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F27" s="3"/>
     </row>
@@ -2229,13 +2256,13 @@
         <v>4.3</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>175</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F28" s="3"/>
     </row>
@@ -2247,10 +2274,10 @@
         <v>45</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>406</v>
+        <v>40</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F29" s="13"/>
     </row>
@@ -2347,7 +2374,7 @@
         <v>64</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F36" s="2"/>
     </row>
@@ -2359,10 +2386,10 @@
         <v>62</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F37" s="2"/>
     </row>
@@ -2374,10 +2401,10 @@
         <v>62</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F38" s="2"/>
     </row>
@@ -2573,7 +2600,7 @@
         <v>72</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F52" s="2"/>
     </row>
@@ -2588,7 +2615,7 @@
         <v>74</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F53" s="2"/>
     </row>
@@ -2835,9 +2862,9 @@
         <v>13.4</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D72" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D72" s="14" t="s">
         <v>91</v>
       </c>
       <c r="E72" s="2" t="s">
@@ -3030,7 +3057,7 @@
         <v>111</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>112</v>
@@ -3060,7 +3087,7 @@
         <v>107</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>108</v>
@@ -4784,7 +4811,7 @@
         <v>234</v>
       </c>
       <c r="E211" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F211" s="2"/>
     </row>
@@ -4793,13 +4820,13 @@
         <v>40.200000000000003</v>
       </c>
       <c r="C212" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D212" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D212" s="2" t="s">
-        <v>240</v>
-      </c>
       <c r="E212" s="2" t="s">
-        <v>241</v>
+        <v>415</v>
       </c>
       <c r="F212" s="2"/>
     </row>
@@ -4814,7 +4841,7 @@
         <v>236</v>
       </c>
       <c r="E213" s="2" t="s">
-        <v>237</v>
+        <v>414</v>
       </c>
       <c r="F213" s="2"/>
     </row>
@@ -4838,7 +4865,7 @@
         <v>41</v>
       </c>
       <c r="C215" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D215" s="7"/>
       <c r="E215" s="7"/>
@@ -4849,11 +4876,11 @@
         <v>41.1</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D216" s="2"/>
       <c r="E216" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F216" s="3"/>
     </row>
@@ -4877,13 +4904,13 @@
         <v>41.3</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D218" s="2" t="s">
         <v>129</v>
       </c>
       <c r="E218" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F218" s="3"/>
     </row>
@@ -4922,7 +4949,7 @@
         <v>42</v>
       </c>
       <c r="C221" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D221" s="7"/>
       <c r="E221" s="7"/>
@@ -4946,13 +4973,13 @@
         <v>42.2</v>
       </c>
       <c r="C223" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D223" s="14" t="s">
         <v>248</v>
       </c>
-      <c r="D223" s="14" t="s">
-        <v>250</v>
-      </c>
       <c r="E223" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F223" s="2"/>
     </row>
@@ -4976,7 +5003,7 @@
         <v>43</v>
       </c>
       <c r="C225" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D225" s="7"/>
       <c r="E225" s="7"/>
@@ -5003,10 +5030,10 @@
         <v>174</v>
       </c>
       <c r="D227" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="E227" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="E227" s="2" t="s">
-        <v>252</v>
       </c>
       <c r="F227" s="2"/>
     </row>
@@ -5030,7 +5057,7 @@
         <v>44</v>
       </c>
       <c r="C229" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D229" s="7"/>
       <c r="E229" s="7"/>
@@ -5041,13 +5068,13 @@
         <v>44.1</v>
       </c>
       <c r="C230" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D230" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E230" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="D230" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="E230" s="2" t="s">
-        <v>256</v>
       </c>
       <c r="F230" s="2"/>
     </row>
@@ -5071,7 +5098,7 @@
         <v>45</v>
       </c>
       <c r="C232" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D232" s="7"/>
       <c r="E232" s="7"/>
@@ -5155,7 +5182,7 @@
         <v>46</v>
       </c>
       <c r="C238" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D238" s="7"/>
       <c r="E238" s="7"/>
@@ -5166,13 +5193,13 @@
         <v>46.1</v>
       </c>
       <c r="C239" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D239" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E239" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="D239" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="E239" s="2" t="s">
-        <v>261</v>
       </c>
       <c r="F239" s="2"/>
     </row>
@@ -5181,13 +5208,13 @@
         <v>46.2</v>
       </c>
       <c r="C240" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D240" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E240" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="D240" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="E240" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="F240" s="2"/>
     </row>
@@ -5196,13 +5223,13 @@
         <v>46.3</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D241" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E241" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="E241" s="2" t="s">
-        <v>265</v>
       </c>
       <c r="F241" s="2"/>
     </row>
@@ -5226,7 +5253,7 @@
         <v>47</v>
       </c>
       <c r="C243" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D243" s="7"/>
       <c r="E243" s="7"/>
@@ -5310,7 +5337,7 @@
         <v>48</v>
       </c>
       <c r="C249" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D249" s="7"/>
       <c r="E249" s="7"/>
@@ -5321,13 +5348,13 @@
         <v>48.1</v>
       </c>
       <c r="C250" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D250" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="E250" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="D250" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="E250" s="2" t="s">
-        <v>271</v>
       </c>
       <c r="F250" s="2"/>
     </row>
@@ -5336,13 +5363,13 @@
         <v>48.2</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E251" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F251" s="2"/>
     </row>
@@ -5351,13 +5378,13 @@
         <v>48.3</v>
       </c>
       <c r="C252" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D252" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E252" s="2" t="s">
         <v>274</v>
-      </c>
-      <c r="D252" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="E252" s="2" t="s">
-        <v>276</v>
       </c>
       <c r="F252" s="2"/>
     </row>
@@ -5381,7 +5408,7 @@
         <v>49</v>
       </c>
       <c r="C254" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D254" s="7"/>
       <c r="E254" s="7"/>
@@ -5420,13 +5447,13 @@
         <v>49.3</v>
       </c>
       <c r="C257" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D257" s="2" t="s">
         <v>129</v>
       </c>
       <c r="E257" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F257" s="3"/>
     </row>
@@ -5465,7 +5492,7 @@
         <v>50</v>
       </c>
       <c r="C260" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D260" s="7"/>
       <c r="E260" s="7"/>
@@ -5476,13 +5503,13 @@
         <v>50.1</v>
       </c>
       <c r="C261" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D261" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E261" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="D261" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="E261" s="2" t="s">
-        <v>283</v>
       </c>
       <c r="F261" s="2"/>
     </row>
@@ -5491,13 +5518,13 @@
         <v>50.2</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D262" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E262" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F262" s="2"/>
     </row>
@@ -5506,13 +5533,13 @@
         <v>50.3</v>
       </c>
       <c r="C263" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D263" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E263" s="2" t="s">
         <v>274</v>
-      </c>
-      <c r="D263" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="E263" s="2" t="s">
-        <v>276</v>
       </c>
       <c r="F263" s="2"/>
     </row>
@@ -5536,7 +5563,7 @@
         <v>51</v>
       </c>
       <c r="C265" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D265" s="7"/>
       <c r="E265" s="7"/>
@@ -5547,11 +5574,11 @@
         <v>51.1</v>
       </c>
       <c r="C266" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D266" s="2"/>
       <c r="E266" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F266" s="2"/>
     </row>
@@ -5560,11 +5587,11 @@
         <v>51.2</v>
       </c>
       <c r="C267" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D267" s="2"/>
       <c r="E267" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F267" s="2"/>
     </row>
@@ -5573,11 +5600,11 @@
         <v>51.3</v>
       </c>
       <c r="C268" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D268" s="2"/>
       <c r="E268" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F268" s="2"/>
     </row>
@@ -5586,11 +5613,11 @@
         <v>51.4</v>
       </c>
       <c r="C269" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D269" s="2"/>
       <c r="E269" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F269" s="2"/>
     </row>
@@ -5599,11 +5626,11 @@
         <v>51.5</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D270" s="2"/>
       <c r="E270" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F270" s="2"/>
     </row>
@@ -5612,11 +5639,11 @@
         <v>51.6</v>
       </c>
       <c r="C271" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D271" s="2"/>
       <c r="E271" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F271" s="2"/>
     </row>
@@ -5625,11 +5652,11 @@
         <v>51.7</v>
       </c>
       <c r="C272" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D272" s="2"/>
       <c r="E272" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F272" s="2"/>
     </row>
@@ -5638,11 +5665,11 @@
         <v>51.8</v>
       </c>
       <c r="C273" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D273" s="2"/>
       <c r="E273" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F273" s="2"/>
     </row>
@@ -5666,7 +5693,7 @@
         <v>52</v>
       </c>
       <c r="C275" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D275" s="7"/>
       <c r="E275" s="7"/>
@@ -5677,11 +5704,11 @@
         <v>52.1</v>
       </c>
       <c r="C276" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D276" s="2"/>
       <c r="E276" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F276" s="2"/>
     </row>
@@ -5690,11 +5717,11 @@
         <v>52.2</v>
       </c>
       <c r="C277" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D277" s="2"/>
       <c r="E277" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F277" s="2"/>
     </row>
@@ -5703,11 +5730,11 @@
         <v>52.3</v>
       </c>
       <c r="C278" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D278" s="2"/>
       <c r="E278" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F278" s="2"/>
     </row>
@@ -5731,7 +5758,7 @@
         <v>53</v>
       </c>
       <c r="C280" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D280" s="7"/>
       <c r="E280" s="7"/>
@@ -5742,11 +5769,11 @@
         <v>53.1</v>
       </c>
       <c r="C281" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D281" s="2"/>
       <c r="E281" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F281" s="2"/>
     </row>
@@ -5770,7 +5797,7 @@
         <v>54</v>
       </c>
       <c r="C283" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D283" s="7"/>
       <c r="E283" s="7"/>
@@ -5781,13 +5808,13 @@
         <v>54.1</v>
       </c>
       <c r="C284" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D284" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="D284" s="2" t="s">
+      <c r="E284" s="2" t="s">
         <v>329</v>
-      </c>
-      <c r="E284" s="2" t="s">
-        <v>330</v>
       </c>
       <c r="F284" s="2"/>
     </row>
@@ -5811,7 +5838,7 @@
         <v>55</v>
       </c>
       <c r="C286" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D286" s="7"/>
       <c r="E286" s="7"/>
@@ -5822,11 +5849,11 @@
         <v>55.1</v>
       </c>
       <c r="C287" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D287" s="2"/>
       <c r="E287" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F287" s="3"/>
     </row>
@@ -5841,7 +5868,7 @@
         <v>127</v>
       </c>
       <c r="E288" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F288" s="3"/>
     </row>
@@ -5850,13 +5877,13 @@
         <v>55.3</v>
       </c>
       <c r="C289" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D289" s="2" t="s">
         <v>129</v>
       </c>
       <c r="E289" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F289" s="3"/>
     </row>
@@ -5871,7 +5898,7 @@
         <v>139</v>
       </c>
       <c r="E290" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F290" s="3"/>
     </row>
@@ -5895,7 +5922,7 @@
         <v>56</v>
       </c>
       <c r="C292" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D292" s="7"/>
       <c r="E292" s="7"/>
@@ -5919,13 +5946,13 @@
         <v>56.2</v>
       </c>
       <c r="C294" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="D294" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="E294" s="2" t="s">
         <v>338</v>
-      </c>
-      <c r="D294" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="E294" s="2" t="s">
-        <v>339</v>
       </c>
       <c r="F294" s="2"/>
     </row>
@@ -5934,13 +5961,13 @@
         <v>56.3</v>
       </c>
       <c r="C295" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="D295" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="E295" s="2" t="s">
         <v>340</v>
-      </c>
-      <c r="D295" s="12" t="s">
-        <v>348</v>
-      </c>
-      <c r="E295" s="2" t="s">
-        <v>341</v>
       </c>
       <c r="F295" s="2"/>
     </row>
@@ -5964,7 +5991,7 @@
         <v>57</v>
       </c>
       <c r="C297" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D297" s="7"/>
       <c r="E297" s="7"/>
@@ -5988,13 +6015,13 @@
         <v>57.2</v>
       </c>
       <c r="C299" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="D299" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E299" s="2" t="s">
         <v>338</v>
-      </c>
-      <c r="D299" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="E299" s="2" t="s">
-        <v>339</v>
       </c>
       <c r="F299" s="2"/>
     </row>
@@ -6006,10 +6033,10 @@
         <v>174</v>
       </c>
       <c r="D300" s="12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E300" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F300" s="2"/>
     </row>
@@ -6033,7 +6060,7 @@
         <v>58</v>
       </c>
       <c r="C302" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D302" s="7"/>
       <c r="E302" s="7"/>
@@ -6044,13 +6071,13 @@
         <v>58.1</v>
       </c>
       <c r="C303" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D303" s="2" t="s">
         <v>211</v>
       </c>
       <c r="E303" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F303" s="2"/>
     </row>
@@ -6074,7 +6101,7 @@
         <v>59</v>
       </c>
       <c r="C305" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D305" s="7"/>
       <c r="E305" s="7"/>
@@ -6085,11 +6112,11 @@
         <v>59.1</v>
       </c>
       <c r="C306" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D306" s="2"/>
       <c r="E306" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F306" s="3"/>
     </row>
@@ -6104,7 +6131,7 @@
         <v>127</v>
       </c>
       <c r="E307" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F307" s="3"/>
     </row>
@@ -6113,13 +6140,13 @@
         <v>59.3</v>
       </c>
       <c r="C308" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D308" s="2" t="s">
         <v>129</v>
       </c>
       <c r="E308" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F308" s="3"/>
     </row>
@@ -6134,7 +6161,7 @@
         <v>139</v>
       </c>
       <c r="E309" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F309" s="3"/>
     </row>
@@ -6158,7 +6185,7 @@
         <v>60</v>
       </c>
       <c r="C311" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D311" s="7"/>
       <c r="E311" s="7"/>
@@ -6169,13 +6196,13 @@
         <v>60.1</v>
       </c>
       <c r="C312" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D312" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E312" s="2" t="s">
         <v>354</v>
-      </c>
-      <c r="D312" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="E312" s="2" t="s">
-        <v>355</v>
       </c>
       <c r="F312" s="2"/>
     </row>
@@ -6190,7 +6217,7 @@
         <v>127</v>
       </c>
       <c r="E313" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F313" s="3"/>
     </row>
@@ -6199,13 +6226,13 @@
         <v>60.3</v>
       </c>
       <c r="C314" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D314" s="2" t="s">
         <v>129</v>
       </c>
       <c r="E314" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F314" s="3"/>
     </row>
@@ -6220,7 +6247,7 @@
         <v>139</v>
       </c>
       <c r="E315" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F315" s="3"/>
     </row>
@@ -6259,7 +6286,7 @@
         <v>61</v>
       </c>
       <c r="C318" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D318" s="7"/>
       <c r="E318" s="7"/>
@@ -6270,11 +6297,11 @@
         <v>61.1</v>
       </c>
       <c r="C319" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D319" s="3"/>
       <c r="E319" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F319" s="2"/>
     </row>
@@ -6283,13 +6310,13 @@
         <v>61.2</v>
       </c>
       <c r="C320" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="D320" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="D320" s="3" t="s">
-        <v>373</v>
-      </c>
       <c r="E320" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F320" s="2"/>
     </row>
@@ -6298,11 +6325,11 @@
         <v>61.3</v>
       </c>
       <c r="C321" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D321" s="3"/>
       <c r="E321" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F321" s="2"/>
     </row>
@@ -6311,13 +6338,13 @@
         <v>61.4</v>
       </c>
       <c r="C322" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D322" s="21">
         <v>0</v>
       </c>
       <c r="E322" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F322" s="2"/>
     </row>
@@ -6326,13 +6353,13 @@
         <v>61.5</v>
       </c>
       <c r="C323" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="D323" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="D323" s="3" t="s">
+      <c r="E323" s="2" t="s">
         <v>367</v>
-      </c>
-      <c r="E323" s="2" t="s">
-        <v>368</v>
       </c>
       <c r="F323" s="2"/>
     </row>
@@ -6356,7 +6383,7 @@
         <v>62</v>
       </c>
       <c r="C325" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D325" s="7"/>
       <c r="E325" s="7"/>
@@ -6367,11 +6394,11 @@
         <v>62.1</v>
       </c>
       <c r="C326" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D326" s="3"/>
       <c r="E326" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F326" s="2" t="s">
         <v>75</v>
@@ -6382,13 +6409,13 @@
         <v>62.2</v>
       </c>
       <c r="C327" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="D327" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="D327" s="3" t="s">
-        <v>373</v>
-      </c>
       <c r="E327" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F327" s="2"/>
     </row>
@@ -6397,11 +6424,11 @@
         <v>62.3</v>
       </c>
       <c r="C328" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D328" s="3"/>
       <c r="E328" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F328" s="2" t="s">
         <v>75</v>
@@ -6412,13 +6439,13 @@
         <v>62.4</v>
       </c>
       <c r="C329" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D329" s="21">
         <v>0</v>
       </c>
       <c r="E329" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F329" s="2"/>
     </row>
@@ -6427,13 +6454,13 @@
         <v>62.5</v>
       </c>
       <c r="C330" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D330" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E330" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F330" s="2"/>
     </row>
@@ -6457,7 +6484,7 @@
         <v>63</v>
       </c>
       <c r="C332" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D332" s="7"/>
       <c r="E332" s="7"/>
@@ -6468,13 +6495,13 @@
         <v>63.1</v>
       </c>
       <c r="C333" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D333" s="2" t="s">
         <v>211</v>
       </c>
       <c r="E333" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F333" s="2"/>
     </row>
@@ -6498,7 +6525,7 @@
         <v>64</v>
       </c>
       <c r="C335" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D335" s="7"/>
       <c r="E335" s="7"/>
@@ -6509,11 +6536,11 @@
         <v>64.099999999999994</v>
       </c>
       <c r="C336" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D336" s="2"/>
       <c r="E336" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F336" s="3"/>
     </row>
@@ -6528,7 +6555,7 @@
         <v>127</v>
       </c>
       <c r="E337" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F337" s="3"/>
     </row>
@@ -6537,13 +6564,13 @@
         <v>64.3</v>
       </c>
       <c r="C338" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D338" s="2" t="s">
         <v>129</v>
       </c>
       <c r="E338" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F338" s="3"/>
     </row>
@@ -6558,7 +6585,7 @@
         <v>139</v>
       </c>
       <c r="E339" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F339" s="3"/>
     </row>
@@ -6582,7 +6609,7 @@
         <v>65</v>
       </c>
       <c r="C341" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D341" s="7"/>
       <c r="E341" s="7"/>
@@ -6606,13 +6633,13 @@
         <v>65.2</v>
       </c>
       <c r="C343" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D343" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E343" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F343" s="2"/>
     </row>
@@ -6621,13 +6648,13 @@
         <v>65.3</v>
       </c>
       <c r="C344" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="D344" s="22" t="s">
+        <v>392</v>
+      </c>
+      <c r="E344" s="2" t="s">
         <v>391</v>
-      </c>
-      <c r="D344" s="22" t="s">
-        <v>393</v>
-      </c>
-      <c r="E344" s="2" t="s">
-        <v>392</v>
       </c>
       <c r="F344" s="2"/>
     </row>
@@ -6636,16 +6663,16 @@
         <v>65.400000000000006</v>
       </c>
       <c r="C345" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D345" s="22" t="s">
         <v>394</v>
       </c>
-      <c r="D345" s="22" t="s">
+      <c r="E345" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="E345" s="2" t="s">
+      <c r="F345" s="2" t="s">
         <v>396</v>
-      </c>
-      <c r="F345" s="2" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="346" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6653,13 +6680,13 @@
         <v>65.5</v>
       </c>
       <c r="C346" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="D346" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="E346" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="D346" s="12" t="s">
-        <v>398</v>
-      </c>
-      <c r="E346" s="2" t="s">
-        <v>385</v>
       </c>
       <c r="F346" s="2"/>
     </row>
@@ -6683,7 +6710,7 @@
         <v>66</v>
       </c>
       <c r="C348" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D348" s="7"/>
       <c r="E348" s="7"/>
@@ -6707,13 +6734,13 @@
         <v>66.2</v>
       </c>
       <c r="C350" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D350" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E350" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F350" s="2"/>
     </row>
@@ -6722,13 +6749,13 @@
         <v>66.3</v>
       </c>
       <c r="C351" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="D351" s="22" t="s">
+        <v>392</v>
+      </c>
+      <c r="E351" s="2" t="s">
         <v>391</v>
-      </c>
-      <c r="D351" s="22" t="s">
-        <v>393</v>
-      </c>
-      <c r="E351" s="2" t="s">
-        <v>392</v>
       </c>
       <c r="F351" s="2"/>
     </row>
@@ -6737,16 +6764,16 @@
         <v>66.400000000000006</v>
       </c>
       <c r="C352" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D352" s="22" t="s">
         <v>394</v>
       </c>
-      <c r="D352" s="22" t="s">
+      <c r="E352" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="E352" s="2" t="s">
+      <c r="F352" s="2" t="s">
         <v>396</v>
-      </c>
-      <c r="F352" s="2" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="353" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6754,13 +6781,13 @@
         <v>66.5</v>
       </c>
       <c r="C353" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D353" s="12" t="s">
         <v>400</v>
       </c>
-      <c r="D353" s="12" t="s">
+      <c r="E353" s="2" t="s">
         <v>401</v>
-      </c>
-      <c r="E353" s="2" t="s">
-        <v>402</v>
       </c>
       <c r="F353" s="2"/>
     </row>
@@ -6784,7 +6811,7 @@
         <v>67</v>
       </c>
       <c r="C355" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D355" s="7"/>
       <c r="E355" s="7"/>
@@ -6795,13 +6822,13 @@
         <v>67.099999999999994</v>
       </c>
       <c r="C356" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D356" s="2" t="s">
         <v>211</v>
       </c>
       <c r="E356" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F356" s="2"/>
     </row>
@@ -6819,6 +6846,90 @@
         <v>11</v>
       </c>
       <c r="F357" s="3"/>
+    </row>
+    <row r="358" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B358" s="8">
+        <v>68</v>
+      </c>
+      <c r="C358" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="D358" s="7"/>
+      <c r="E358" s="7"/>
+      <c r="F358" s="7"/>
+    </row>
+    <row r="359" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B359" s="10">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="C359" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D359" s="2"/>
+      <c r="E359" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="F359" s="2"/>
+    </row>
+    <row r="360" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B360" s="10">
+        <v>68.2</v>
+      </c>
+      <c r="C360" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="D360" s="23">
+        <v>44936</v>
+      </c>
+      <c r="E360" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="F360" s="2"/>
+    </row>
+    <row r="361" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B361" s="10">
+        <v>68.3</v>
+      </c>
+      <c r="C361" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="D361" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="E361" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="F361" s="2"/>
+    </row>
+    <row r="362" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B362" s="10">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="C362" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="D362" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="E362" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="F362" s="2"/>
+    </row>
+    <row r="363" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B363" s="10">
+        <v>68.5</v>
+      </c>
+      <c r="C363" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D363" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E363" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F363" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>